<commit_message>
Format column was being used wrong.
</commit_message>
<xml_diff>
--- a/ExampleProject/example_sdd.xlsx
+++ b/ExampleProject/example_sdd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmccusker/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F6404F-F890-AD4F-9797-D87886B4692F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE67985E-F8EB-1C48-BA8F-2BEB9D631F8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15600" yWindow="2880" windowWidth="21540" windowHeight="16920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5060" yWindow="4420" windowWidth="28160" windowHeight="19340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InfoSheet" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="1554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="1554">
   <si>
     <t>Attribute</t>
   </si>
@@ -2670,9 +2670,6 @@
     <t>Weight of the subject in kilograms at visit 2</t>
   </si>
   <si>
-    <t>decimal</t>
-  </si>
-  <si>
     <t>wt2-{id}</t>
   </si>
   <si>
@@ -4687,6 +4684,9 @@
   </si>
   <si>
     <t>url</t>
+  </si>
+  <si>
+    <t>xsd:integer</t>
   </si>
 </sst>
 </file>
@@ -5143,7 +5143,7 @@
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>858</v>
@@ -5180,7 +5180,7 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -5188,10 +5188,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>1551</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1552</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1553</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5343,11 +5343,11 @@
   </sheetPr>
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="331" zoomScaleNormal="331" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:A1048576"/>
+      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5506,7 +5506,7 @@
         <v>53</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>881</v>
+        <v>875</v>
       </c>
       <c r="I4" s="11" t="s">
         <v>58</v>
@@ -5518,7 +5518,7 @@
       <c r="N4" s="11"/>
       <c r="O4" s="11"/>
       <c r="P4" s="11" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5526,13 +5526,13 @@
         <v>47</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>882</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>883</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="D5" s="11" t="s">
         <v>884</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>885</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>48</v>
@@ -5541,9 +5541,11 @@
         <v>863</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>886</v>
-      </c>
-      <c r="H5" s="11"/>
+        <v>885</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>1553</v>
+      </c>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
@@ -5552,24 +5554,24 @@
       <c r="N5" s="11"/>
       <c r="O5" s="11"/>
       <c r="P5" s="11" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
+        <v>887</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>888</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="C6" s="11" t="s">
         <v>889</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="D6" s="11" t="s">
         <v>890</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="E6" s="11" t="s">
         <v>891</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>892</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>863</v>
@@ -5584,7 +5586,7 @@
       <c r="N6" s="11"/>
       <c r="O6" s="11"/>
       <c r="P6" s="11" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5592,16 +5594,16 @@
         <v>46</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>893</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>894</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>895</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="E7" s="11" t="s">
         <v>896</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>897</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>863</v>
@@ -5616,7 +5618,7 @@
       <c r="N7" s="11"/>
       <c r="O7" s="11"/>
       <c r="P7" s="11" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5624,13 +5626,13 @@
         <v>50</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>898</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>899</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="D8" s="11" t="s">
         <v>900</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>901</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>51</v>
@@ -5648,7 +5650,7 @@
       <c r="N8" s="11"/>
       <c r="O8" s="11"/>
       <c r="P8" s="11" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5656,13 +5658,13 @@
         <v>72</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>902</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>903</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="D9" s="11" t="s">
         <v>904</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>905</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>56</v>
@@ -5680,7 +5682,7 @@
       <c r="N9" s="11"/>
       <c r="O9" s="11"/>
       <c r="P9" s="11" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5688,13 +5690,13 @@
         <v>863</v>
       </c>
       <c r="B10" s="11" t="s">
+        <v>906</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>907</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="D10" s="11" t="s">
         <v>908</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>909</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
@@ -5705,7 +5707,7 @@
         <v>61</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="L10" s="11"/>
       <c r="M10" s="11" t="s">
@@ -5714,7 +5716,7 @@
       <c r="N10" s="11"/>
       <c r="O10" s="11"/>
       <c r="P10" s="11" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5722,10 +5724,10 @@
         <v>45</v>
       </c>
       <c r="B11" s="11" t="s">
+        <v>911</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>912</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>913</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
@@ -5734,7 +5736,7 @@
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
       <c r="J11" s="11" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
@@ -5742,7 +5744,7 @@
       <c r="N11" s="11"/>
       <c r="O11" s="11"/>
       <c r="P11" s="11" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5861,32 +5863,32 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5901,7 +5903,7 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5912,11 +5914,11 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5927,11 +5929,11 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5942,11 +5944,11 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5957,11 +5959,11 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5976,7 +5978,7 @@
       </c>
       <c r="D9" s="3"/>
       <c r="E9" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5990,7 +5992,7 @@
         <v>70</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6001,10 +6003,10 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
+        <v>930</v>
+      </c>
+      <c r="E11" t="s">
         <v>931</v>
-      </c>
-      <c r="E11" t="s">
-        <v>932</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6018,7 +6020,7 @@
         <v>71</v>
       </c>
       <c r="E12" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6029,10 +6031,10 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
+        <v>933</v>
+      </c>
+      <c r="E13" t="s">
         <v>934</v>
-      </c>
-      <c r="E13" t="s">
-        <v>935</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6046,7 +6048,7 @@
         <v>73</v>
       </c>
       <c r="E14" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6122,13 +6124,13 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
+        <v>936</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>937</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>938</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>939</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -6156,13 +6158,13 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
+        <v>939</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>940</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>941</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>942</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -6190,13 +6192,13 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
+        <v>942</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>943</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>944</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>945</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -6224,13 +6226,13 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
+        <v>945</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>946</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>947</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>948</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -6258,13 +6260,13 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
+        <v>948</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>949</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>950</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>951</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -6292,13 +6294,13 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
+        <v>951</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>952</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>953</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>954</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -6326,13 +6328,13 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
+        <v>954</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>955</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>956</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>957</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -6360,13 +6362,13 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
+        <v>957</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>958</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>959</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>960</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -6394,13 +6396,13 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
+        <v>960</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>961</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>962</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>963</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -6496,13 +6498,13 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
+        <v>963</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>964</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>965</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>966</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -6632,13 +6634,13 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
+        <v>966</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>967</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>968</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>969</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -6734,13 +6736,13 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
+        <v>969</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>970</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>971</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>972</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -6802,13 +6804,13 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
+        <v>972</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>973</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -7074,13 +7076,13 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
+        <v>975</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>976</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>977</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>978</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -7822,13 +7824,13 @@
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
+        <v>978</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>979</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="C52" s="5" t="s">
         <v>980</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>981</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
@@ -8026,13 +8028,13 @@
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
+        <v>981</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>982</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="C58" s="5" t="s">
         <v>983</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>984</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
@@ -8128,13 +8130,13 @@
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
+        <v>984</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>985</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="C61" s="5" t="s">
         <v>986</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>987</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
@@ -8230,13 +8232,13 @@
     </row>
     <row r="64" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
+        <v>987</v>
+      </c>
+      <c r="B64" s="5" t="s">
         <v>988</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="C64" s="5" t="s">
         <v>989</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>990</v>
       </c>
       <c r="D64" s="6"/>
       <c r="E64" s="6"/>
@@ -8332,13 +8334,13 @@
     </row>
     <row r="67" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
+        <v>990</v>
+      </c>
+      <c r="B67" s="5" t="s">
         <v>991</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="C67" s="5" t="s">
         <v>992</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>993</v>
       </c>
       <c r="D67" s="6"/>
       <c r="E67" s="6"/>
@@ -8400,13 +8402,13 @@
     </row>
     <row r="69" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
+        <v>993</v>
+      </c>
+      <c r="B69" s="5" t="s">
         <v>994</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="C69" s="5" t="s">
         <v>995</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>996</v>
       </c>
       <c r="D69" s="6"/>
       <c r="E69" s="6"/>
@@ -8434,13 +8436,13 @@
     </row>
     <row r="70" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
+        <v>996</v>
+      </c>
+      <c r="B70" s="5" t="s">
         <v>997</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="C70" s="5" t="s">
         <v>998</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>999</v>
       </c>
       <c r="D70" s="6"/>
       <c r="E70" s="6"/>
@@ -8536,13 +8538,13 @@
     </row>
     <row r="73" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
+        <v>999</v>
+      </c>
+      <c r="B73" s="5" t="s">
         <v>1000</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="C73" s="5" t="s">
         <v>1001</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>1002</v>
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="6"/>
@@ -8570,13 +8572,13 @@
     </row>
     <row r="74" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B74" s="5" t="s">
         <v>1003</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="C74" s="5" t="s">
         <v>1004</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>1005</v>
       </c>
       <c r="D74" s="6"/>
       <c r="E74" s="6"/>
@@ -8638,13 +8640,13 @@
     </row>
     <row r="76" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B76" s="5" t="s">
         <v>1006</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="C76" s="5" t="s">
         <v>1007</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>1008</v>
       </c>
       <c r="D76" s="6"/>
       <c r="E76" s="6"/>
@@ -8842,13 +8844,13 @@
     </row>
     <row r="82" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B82" s="5" t="s">
         <v>1009</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="C82" s="5" t="s">
         <v>1010</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>1011</v>
       </c>
       <c r="D82" s="6"/>
       <c r="E82" s="6"/>
@@ -8882,7 +8884,7 @@
         <v>846</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="D83" s="6"/>
       <c r="E83" s="6"/>
@@ -8910,13 +8912,13 @@
     </row>
     <row r="84" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B84" s="5" t="s">
         <v>1013</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="C84" s="5" t="s">
         <v>1014</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>1015</v>
       </c>
       <c r="D84" s="6"/>
       <c r="E84" s="6"/>
@@ -8944,13 +8946,13 @@
     </row>
     <row r="85" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B85" s="5" t="s">
         <v>1016</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="C85" s="5" t="s">
         <v>1017</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>1018</v>
       </c>
       <c r="D85" s="6"/>
       <c r="E85" s="6"/>
@@ -8978,13 +8980,13 @@
     </row>
     <row r="86" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B86" s="5" t="s">
         <v>1019</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="C86" s="5" t="s">
         <v>1020</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>1021</v>
       </c>
       <c r="D86" s="6"/>
       <c r="E86" s="6"/>
@@ -9012,13 +9014,13 @@
     </row>
     <row r="87" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B87" s="5" t="s">
         <v>1022</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="C87" s="5" t="s">
         <v>1023</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>1024</v>
       </c>
       <c r="D87" s="6"/>
       <c r="E87" s="6"/>
@@ -9148,13 +9150,13 @@
     </row>
     <row r="91" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B91" s="5" t="s">
         <v>1025</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="C91" s="5" t="s">
         <v>1026</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>1027</v>
       </c>
       <c r="D91" s="6"/>
       <c r="E91" s="6"/>
@@ -9182,13 +9184,13 @@
     </row>
     <row r="92" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B92" s="5" t="s">
         <v>1028</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="C92" s="5" t="s">
         <v>1029</v>
-      </c>
-      <c r="C92" s="5" t="s">
-        <v>1030</v>
       </c>
       <c r="D92" s="6"/>
       <c r="E92" s="6"/>
@@ -9216,13 +9218,13 @@
     </row>
     <row r="93" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B93" s="5" t="s">
         <v>1031</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="C93" s="5" t="s">
         <v>1032</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>1033</v>
       </c>
       <c r="D93" s="6"/>
       <c r="E93" s="6"/>
@@ -9250,13 +9252,13 @@
     </row>
     <row r="94" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B94" s="5" t="s">
         <v>1034</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="C94" s="5" t="s">
         <v>1035</v>
-      </c>
-      <c r="C94" s="5" t="s">
-        <v>1036</v>
       </c>
       <c r="D94" s="6"/>
       <c r="E94" s="6"/>
@@ -9488,13 +9490,13 @@
     </row>
     <row r="101" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B101" s="5" t="s">
         <v>1037</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="C101" s="5" t="s">
         <v>1038</v>
-      </c>
-      <c r="C101" s="5" t="s">
-        <v>1039</v>
       </c>
       <c r="D101" s="6"/>
       <c r="E101" s="6"/>
@@ -9590,13 +9592,13 @@
     </row>
     <row r="104" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A104" s="12" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B104" s="5" t="s">
         <v>1040</v>
       </c>
-      <c r="B104" s="5" t="s">
+      <c r="C104" s="5" t="s">
         <v>1041</v>
-      </c>
-      <c r="C104" s="5" t="s">
-        <v>1042</v>
       </c>
       <c r="D104" s="6"/>
       <c r="E104" s="6"/>
@@ -9624,13 +9626,13 @@
     </row>
     <row r="105" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A105" s="12" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B105" s="5" t="s">
         <v>1043</v>
       </c>
-      <c r="B105" s="5" t="s">
+      <c r="C105" s="5" t="s">
         <v>1044</v>
-      </c>
-      <c r="C105" s="5" t="s">
-        <v>1045</v>
       </c>
       <c r="D105" s="6"/>
       <c r="E105" s="6"/>
@@ -9998,13 +10000,13 @@
     </row>
     <row r="116" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A116" s="12" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B116" s="5" t="s">
         <v>1046</v>
       </c>
-      <c r="B116" s="5" t="s">
+      <c r="C116" s="5" t="s">
         <v>1047</v>
-      </c>
-      <c r="C116" s="5" t="s">
-        <v>1048</v>
       </c>
       <c r="D116" s="6"/>
       <c r="E116" s="6"/>
@@ -10032,13 +10034,13 @@
     </row>
     <row r="117" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A117" s="12" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B117" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="B117" s="5" t="s">
+      <c r="C117" s="5" t="s">
         <v>1050</v>
-      </c>
-      <c r="C117" s="5" t="s">
-        <v>1051</v>
       </c>
       <c r="D117" s="6"/>
       <c r="E117" s="6"/>
@@ -10066,7 +10068,7 @@
     </row>
     <row r="118" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A118" s="12" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B118" s="5" t="s">
         <v>327</v>
@@ -10202,13 +10204,13 @@
     </row>
     <row r="122" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A122" s="12" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B122" s="5" t="s">
         <v>1053</v>
       </c>
-      <c r="B122" s="5" t="s">
+      <c r="C122" s="5" t="s">
         <v>1054</v>
-      </c>
-      <c r="C122" s="5" t="s">
-        <v>1055</v>
       </c>
       <c r="D122" s="6"/>
       <c r="E122" s="6"/>
@@ -10236,13 +10238,13 @@
     </row>
     <row r="123" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A123" s="12" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B123" s="5" t="s">
         <v>1056</v>
       </c>
-      <c r="B123" s="5" t="s">
+      <c r="C123" s="5" t="s">
         <v>1057</v>
-      </c>
-      <c r="C123" s="5" t="s">
-        <v>1058</v>
       </c>
       <c r="D123" s="6"/>
       <c r="E123" s="6"/>
@@ -10304,13 +10306,13 @@
     </row>
     <row r="125" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A125" s="12" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B125" s="5" t="s">
         <v>1059</v>
       </c>
-      <c r="B125" s="5" t="s">
+      <c r="C125" s="5" t="s">
         <v>1060</v>
-      </c>
-      <c r="C125" s="5" t="s">
-        <v>1061</v>
       </c>
       <c r="D125" s="6"/>
       <c r="E125" s="6"/>
@@ -10338,13 +10340,13 @@
     </row>
     <row r="126" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A126" s="12" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B126" s="5" t="s">
         <v>1062</v>
       </c>
-      <c r="B126" s="5" t="s">
+      <c r="C126" s="5" t="s">
         <v>1063</v>
-      </c>
-      <c r="C126" s="5" t="s">
-        <v>1064</v>
       </c>
       <c r="D126" s="6"/>
       <c r="E126" s="6"/>
@@ -10406,13 +10408,13 @@
     </row>
     <row r="128" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A128" s="12" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B128" s="5" t="s">
         <v>1065</v>
       </c>
-      <c r="B128" s="5" t="s">
+      <c r="C128" s="5" t="s">
         <v>1066</v>
-      </c>
-      <c r="C128" s="5" t="s">
-        <v>1067</v>
       </c>
       <c r="D128" s="6"/>
       <c r="E128" s="6"/>
@@ -10440,13 +10442,13 @@
     </row>
     <row r="129" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A129" s="12" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B129" s="5" t="s">
         <v>1068</v>
       </c>
-      <c r="B129" s="5" t="s">
+      <c r="C129" s="5" t="s">
         <v>1069</v>
-      </c>
-      <c r="C129" s="5" t="s">
-        <v>1070</v>
       </c>
       <c r="D129" s="6"/>
       <c r="E129" s="6"/>
@@ -10474,13 +10476,13 @@
     </row>
     <row r="130" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A130" s="12" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B130" s="5" t="s">
         <v>1071</v>
       </c>
-      <c r="B130" s="5" t="s">
-        <v>1072</v>
-      </c>
       <c r="C130" s="5" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="D130" s="6"/>
       <c r="E130" s="6"/>
@@ -10542,13 +10544,13 @@
     </row>
     <row r="132" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A132" s="12" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B132" s="5" t="s">
         <v>1073</v>
       </c>
-      <c r="B132" s="5" t="s">
+      <c r="C132" s="5" t="s">
         <v>1074</v>
-      </c>
-      <c r="C132" s="5" t="s">
-        <v>1075</v>
       </c>
       <c r="D132" s="6"/>
       <c r="E132" s="6"/>
@@ -10576,13 +10578,13 @@
     </row>
     <row r="133" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A133" s="12" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B133" s="5" t="s">
         <v>1076</v>
       </c>
-      <c r="B133" s="5" t="s">
+      <c r="C133" s="5" t="s">
         <v>1077</v>
-      </c>
-      <c r="C133" s="5" t="s">
-        <v>1078</v>
       </c>
       <c r="D133" s="6"/>
       <c r="E133" s="6"/>
@@ -10610,13 +10612,13 @@
     </row>
     <row r="134" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A134" s="12" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B134" s="5" t="s">
         <v>1079</v>
       </c>
-      <c r="B134" s="5" t="s">
+      <c r="C134" s="5" t="s">
         <v>1080</v>
-      </c>
-      <c r="C134" s="5" t="s">
-        <v>1081</v>
       </c>
       <c r="D134" s="6"/>
       <c r="E134" s="6"/>
@@ -10644,13 +10646,13 @@
     </row>
     <row r="135" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A135" s="12" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B135" s="5" t="s">
         <v>1082</v>
       </c>
-      <c r="B135" s="5" t="s">
+      <c r="C135" s="5" t="s">
         <v>1083</v>
-      </c>
-      <c r="C135" s="5" t="s">
-        <v>1084</v>
       </c>
       <c r="D135" s="6"/>
       <c r="E135" s="6"/>
@@ -10780,13 +10782,13 @@
     </row>
     <row r="139" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A139" s="12" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B139" s="5" t="s">
         <v>1085</v>
       </c>
-      <c r="B139" s="5" t="s">
+      <c r="C139" s="5" t="s">
         <v>1086</v>
-      </c>
-      <c r="C139" s="5" t="s">
-        <v>1087</v>
       </c>
       <c r="D139" s="6"/>
       <c r="E139" s="6"/>
@@ -10814,13 +10816,13 @@
     </row>
     <row r="140" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A140" s="12" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B140" s="5" t="s">
         <v>1088</v>
       </c>
-      <c r="B140" s="5" t="s">
+      <c r="C140" s="5" t="s">
         <v>1089</v>
-      </c>
-      <c r="C140" s="5" t="s">
-        <v>1090</v>
       </c>
       <c r="D140" s="6"/>
       <c r="E140" s="6"/>
@@ -10848,13 +10850,13 @@
     </row>
     <row r="141" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A141" s="12" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B141" s="5" t="s">
         <v>1091</v>
       </c>
-      <c r="B141" s="5" t="s">
+      <c r="C141" s="5" t="s">
         <v>1092</v>
-      </c>
-      <c r="C141" s="5" t="s">
-        <v>1093</v>
       </c>
       <c r="D141" s="6"/>
       <c r="E141" s="6"/>
@@ -10882,13 +10884,13 @@
     </row>
     <row r="142" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A142" s="12" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B142" s="5" t="s">
         <v>1094</v>
       </c>
-      <c r="B142" s="5" t="s">
+      <c r="C142" s="5" t="s">
         <v>1095</v>
-      </c>
-      <c r="C142" s="5" t="s">
-        <v>1096</v>
       </c>
       <c r="D142" s="6"/>
       <c r="E142" s="6"/>
@@ -10916,13 +10918,13 @@
     </row>
     <row r="143" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A143" s="12" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B143" s="5" t="s">
         <v>1097</v>
       </c>
-      <c r="B143" s="5" t="s">
+      <c r="C143" s="5" t="s">
         <v>1098</v>
-      </c>
-      <c r="C143" s="5" t="s">
-        <v>1099</v>
       </c>
       <c r="D143" s="6"/>
       <c r="E143" s="6"/>
@@ -10950,13 +10952,13 @@
     </row>
     <row r="144" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A144" s="12" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B144" s="5" t="s">
         <v>1100</v>
       </c>
-      <c r="B144" s="5" t="s">
+      <c r="C144" s="5" t="s">
         <v>1101</v>
-      </c>
-      <c r="C144" s="5" t="s">
-        <v>1102</v>
       </c>
       <c r="D144" s="6"/>
       <c r="E144" s="6"/>
@@ -10990,7 +10992,7 @@
         <v>844</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="D145" s="6"/>
       <c r="E145" s="6"/>
@@ -11018,13 +11020,13 @@
     </row>
     <row r="146" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A146" s="12" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B146" s="5" t="s">
         <v>1104</v>
       </c>
-      <c r="B146" s="5" t="s">
+      <c r="C146" s="5" t="s">
         <v>1105</v>
-      </c>
-      <c r="C146" s="5" t="s">
-        <v>1106</v>
       </c>
       <c r="D146" s="6"/>
       <c r="E146" s="6"/>
@@ -11052,13 +11054,13 @@
     </row>
     <row r="147" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A147" s="12" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B147" s="5" t="s">
         <v>1107</v>
       </c>
-      <c r="B147" s="5" t="s">
+      <c r="C147" s="5" t="s">
         <v>1108</v>
-      </c>
-      <c r="C147" s="5" t="s">
-        <v>1109</v>
       </c>
       <c r="D147" s="6"/>
       <c r="E147" s="6"/>
@@ -11086,13 +11088,13 @@
     </row>
     <row r="148" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A148" s="12" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B148" s="5" t="s">
         <v>1110</v>
       </c>
-      <c r="B148" s="5" t="s">
+      <c r="C148" s="5" t="s">
         <v>1111</v>
-      </c>
-      <c r="C148" s="5" t="s">
-        <v>1112</v>
       </c>
       <c r="D148" s="6"/>
       <c r="E148" s="6"/>
@@ -11154,13 +11156,13 @@
     </row>
     <row r="150" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A150" s="12" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B150" s="5" t="s">
         <v>1113</v>
       </c>
-      <c r="B150" s="5" t="s">
+      <c r="C150" s="5" t="s">
         <v>1114</v>
-      </c>
-      <c r="C150" s="5" t="s">
-        <v>1115</v>
       </c>
       <c r="D150" s="6"/>
       <c r="E150" s="6"/>
@@ -11188,13 +11190,13 @@
     </row>
     <row r="151" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A151" s="12" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B151" s="5" t="s">
         <v>1116</v>
       </c>
-      <c r="B151" s="5" t="s">
+      <c r="C151" s="5" t="s">
         <v>1117</v>
-      </c>
-      <c r="C151" s="5" t="s">
-        <v>1118</v>
       </c>
       <c r="D151" s="6"/>
       <c r="E151" s="6"/>
@@ -11256,13 +11258,13 @@
     </row>
     <row r="153" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A153" s="12" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B153" s="5" t="s">
         <v>1119</v>
       </c>
-      <c r="B153" s="5" t="s">
+      <c r="C153" s="5" t="s">
         <v>1120</v>
-      </c>
-      <c r="C153" s="5" t="s">
-        <v>1121</v>
       </c>
       <c r="D153" s="6"/>
       <c r="E153" s="6"/>
@@ -11290,13 +11292,13 @@
     </row>
     <row r="154" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A154" s="12" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B154" s="5" t="s">
         <v>1122</v>
       </c>
-      <c r="B154" s="5" t="s">
+      <c r="C154" s="5" t="s">
         <v>1123</v>
-      </c>
-      <c r="C154" s="5" t="s">
-        <v>1124</v>
       </c>
       <c r="D154" s="6"/>
       <c r="E154" s="6"/>
@@ -11664,13 +11666,13 @@
     </row>
     <row r="165" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A165" s="12" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B165" s="5" t="s">
         <v>1125</v>
       </c>
-      <c r="B165" s="5" t="s">
+      <c r="C165" s="5" t="s">
         <v>1126</v>
-      </c>
-      <c r="C165" s="5" t="s">
-        <v>1127</v>
       </c>
       <c r="D165" s="6"/>
       <c r="E165" s="6"/>
@@ -11834,13 +11836,13 @@
     </row>
     <row r="170" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A170" s="12" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B170" s="5" t="s">
         <v>1128</v>
       </c>
-      <c r="B170" s="5" t="s">
+      <c r="C170" s="5" t="s">
         <v>1129</v>
-      </c>
-      <c r="C170" s="5" t="s">
-        <v>1130</v>
       </c>
       <c r="D170" s="6"/>
       <c r="E170" s="6"/>
@@ -11868,13 +11870,13 @@
     </row>
     <row r="171" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A171" s="12" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B171" s="5" t="s">
         <v>1131</v>
       </c>
-      <c r="B171" s="5" t="s">
+      <c r="C171" s="5" t="s">
         <v>1132</v>
-      </c>
-      <c r="C171" s="5" t="s">
-        <v>1133</v>
       </c>
       <c r="D171" s="6"/>
       <c r="E171" s="6"/>
@@ -11902,13 +11904,13 @@
     </row>
     <row r="172" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A172" s="12" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B172" s="5" t="s">
         <v>1134</v>
       </c>
-      <c r="B172" s="5" t="s">
+      <c r="C172" s="5" t="s">
         <v>1135</v>
-      </c>
-      <c r="C172" s="5" t="s">
-        <v>1136</v>
       </c>
       <c r="D172" s="6"/>
       <c r="E172" s="6"/>
@@ -11936,13 +11938,13 @@
     </row>
     <row r="173" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A173" s="12" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B173" s="5" t="s">
         <v>1137</v>
       </c>
-      <c r="B173" s="5" t="s">
+      <c r="C173" s="5" t="s">
         <v>1138</v>
-      </c>
-      <c r="C173" s="5" t="s">
-        <v>1139</v>
       </c>
       <c r="D173" s="6"/>
       <c r="E173" s="6"/>
@@ -11970,13 +11972,13 @@
     </row>
     <row r="174" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A174" s="12" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B174" s="5" t="s">
         <v>1140</v>
       </c>
-      <c r="B174" s="5" t="s">
+      <c r="C174" s="5" t="s">
         <v>1141</v>
-      </c>
-      <c r="C174" s="5" t="s">
-        <v>1142</v>
       </c>
       <c r="D174" s="6"/>
       <c r="E174" s="6"/>
@@ -12004,13 +12006,13 @@
     </row>
     <row r="175" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A175" s="12" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B175" s="5" t="s">
         <v>1143</v>
       </c>
-      <c r="B175" s="5" t="s">
+      <c r="C175" s="5" t="s">
         <v>1144</v>
-      </c>
-      <c r="C175" s="5" t="s">
-        <v>1145</v>
       </c>
       <c r="D175" s="6"/>
       <c r="E175" s="6"/>
@@ -12038,13 +12040,13 @@
     </row>
     <row r="176" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A176" s="12" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B176" s="5" t="s">
         <v>1146</v>
       </c>
-      <c r="B176" s="5" t="s">
+      <c r="C176" s="5" t="s">
         <v>1147</v>
-      </c>
-      <c r="C176" s="5" t="s">
-        <v>1148</v>
       </c>
       <c r="D176" s="6"/>
       <c r="E176" s="6"/>
@@ -12072,13 +12074,13 @@
     </row>
     <row r="177" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A177" s="12" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B177" s="5" t="s">
         <v>1149</v>
       </c>
-      <c r="B177" s="5" t="s">
+      <c r="C177" s="5" t="s">
         <v>1150</v>
-      </c>
-      <c r="C177" s="5" t="s">
-        <v>1151</v>
       </c>
       <c r="D177" s="6"/>
       <c r="E177" s="6"/>
@@ -12112,7 +12114,7 @@
         <v>842</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="D178" s="6"/>
       <c r="E178" s="6"/>
@@ -12140,13 +12142,13 @@
     </row>
     <row r="179" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A179" s="12" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B179" s="5" t="s">
         <v>1153</v>
       </c>
-      <c r="B179" s="5" t="s">
+      <c r="C179" s="5" t="s">
         <v>1154</v>
-      </c>
-      <c r="C179" s="5" t="s">
-        <v>1155</v>
       </c>
       <c r="D179" s="6"/>
       <c r="E179" s="6"/>
@@ -12174,13 +12176,13 @@
     </row>
     <row r="180" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A180" s="12" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B180" s="5" t="s">
         <v>1156</v>
       </c>
-      <c r="B180" s="5" t="s">
+      <c r="C180" s="5" t="s">
         <v>1157</v>
-      </c>
-      <c r="C180" s="5" t="s">
-        <v>1158</v>
       </c>
       <c r="D180" s="6"/>
       <c r="E180" s="6"/>
@@ -12208,13 +12210,13 @@
     </row>
     <row r="181" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A181" s="12" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B181" s="5" t="s">
         <v>1159</v>
       </c>
-      <c r="B181" s="5" t="s">
+      <c r="C181" s="5" t="s">
         <v>1160</v>
-      </c>
-      <c r="C181" s="5" t="s">
-        <v>1161</v>
       </c>
       <c r="D181" s="6"/>
       <c r="E181" s="6"/>
@@ -12245,10 +12247,10 @@
         <v>52</v>
       </c>
       <c r="B182" s="5" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C182" s="5" t="s">
         <v>1162</v>
-      </c>
-      <c r="C182" s="5" t="s">
-        <v>1163</v>
       </c>
       <c r="D182" s="6"/>
       <c r="E182" s="6"/>
@@ -12276,13 +12278,13 @@
     </row>
     <row r="183" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A183" s="12" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B183" s="5" t="s">
         <v>1164</v>
       </c>
-      <c r="B183" s="5" t="s">
+      <c r="C183" s="5" t="s">
         <v>1165</v>
-      </c>
-      <c r="C183" s="5" t="s">
-        <v>1166</v>
       </c>
       <c r="D183" s="6"/>
       <c r="E183" s="6"/>
@@ -12310,13 +12312,13 @@
     </row>
     <row r="184" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A184" s="12" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B184" s="5" t="s">
         <v>1167</v>
       </c>
-      <c r="B184" s="5" t="s">
+      <c r="C184" s="5" t="s">
         <v>1168</v>
-      </c>
-      <c r="C184" s="5" t="s">
-        <v>1169</v>
       </c>
       <c r="D184" s="6"/>
       <c r="E184" s="6"/>
@@ -12344,13 +12346,13 @@
     </row>
     <row r="185" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A185" s="12" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B185" s="5" t="s">
         <v>1170</v>
       </c>
-      <c r="B185" s="5" t="s">
+      <c r="C185" s="5" t="s">
         <v>1171</v>
-      </c>
-      <c r="C185" s="5" t="s">
-        <v>1172</v>
       </c>
       <c r="D185" s="6"/>
       <c r="E185" s="6"/>
@@ -12378,13 +12380,13 @@
     </row>
     <row r="186" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A186" s="12" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B186" s="5" t="s">
         <v>1173</v>
       </c>
-      <c r="B186" s="5" t="s">
+      <c r="C186" s="5" t="s">
         <v>1174</v>
-      </c>
-      <c r="C186" s="5" t="s">
-        <v>1175</v>
       </c>
       <c r="D186" s="6"/>
       <c r="E186" s="6"/>
@@ -12412,13 +12414,13 @@
     </row>
     <row r="187" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A187" s="12" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B187" s="5" t="s">
         <v>1176</v>
       </c>
-      <c r="B187" s="5" t="s">
+      <c r="C187" s="5" t="s">
         <v>1177</v>
-      </c>
-      <c r="C187" s="5" t="s">
-        <v>1178</v>
       </c>
       <c r="D187" s="6"/>
       <c r="E187" s="6"/>
@@ -12446,13 +12448,13 @@
     </row>
     <row r="188" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A188" s="12" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B188" s="5" t="s">
         <v>1179</v>
       </c>
-      <c r="B188" s="5" t="s">
+      <c r="C188" s="5" t="s">
         <v>1180</v>
-      </c>
-      <c r="C188" s="5" t="s">
-        <v>1181</v>
       </c>
       <c r="D188" s="6"/>
       <c r="E188" s="6"/>
@@ -12480,13 +12482,13 @@
     </row>
     <row r="189" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A189" s="12" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B189" s="5" t="s">
         <v>1182</v>
       </c>
-      <c r="B189" s="5" t="s">
+      <c r="C189" s="5" t="s">
         <v>1183</v>
-      </c>
-      <c r="C189" s="5" t="s">
-        <v>1184</v>
       </c>
       <c r="D189" s="6"/>
       <c r="E189" s="6"/>
@@ -12548,13 +12550,13 @@
     </row>
     <row r="191" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A191" s="12" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B191" s="5" t="s">
         <v>1185</v>
       </c>
-      <c r="B191" s="5" t="s">
+      <c r="C191" s="5" t="s">
         <v>1186</v>
-      </c>
-      <c r="C191" s="5" t="s">
-        <v>1187</v>
       </c>
       <c r="D191" s="6"/>
       <c r="E191" s="6"/>
@@ -12582,13 +12584,13 @@
     </row>
     <row r="192" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A192" s="12" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B192" s="5" t="s">
         <v>1188</v>
       </c>
-      <c r="B192" s="5" t="s">
+      <c r="C192" s="5" t="s">
         <v>1189</v>
-      </c>
-      <c r="C192" s="5" t="s">
-        <v>1190</v>
       </c>
       <c r="D192" s="6"/>
       <c r="E192" s="6"/>
@@ -12650,13 +12652,13 @@
     </row>
     <row r="194" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A194" s="12" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B194" s="5" t="s">
         <v>1191</v>
       </c>
-      <c r="B194" s="5" t="s">
+      <c r="C194" s="5" t="s">
         <v>1192</v>
-      </c>
-      <c r="C194" s="5" t="s">
-        <v>1193</v>
       </c>
       <c r="D194" s="6"/>
       <c r="E194" s="6"/>
@@ -12684,13 +12686,13 @@
     </row>
     <row r="195" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A195" s="12" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B195" s="5" t="s">
         <v>1194</v>
       </c>
-      <c r="B195" s="5" t="s">
+      <c r="C195" s="5" t="s">
         <v>1195</v>
-      </c>
-      <c r="C195" s="5" t="s">
-        <v>1196</v>
       </c>
       <c r="D195" s="6"/>
       <c r="E195" s="6"/>
@@ -12718,13 +12720,13 @@
     </row>
     <row r="196" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A196" s="12" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B196" s="5" t="s">
         <v>1197</v>
       </c>
-      <c r="B196" s="5" t="s">
+      <c r="C196" s="5" t="s">
         <v>1198</v>
-      </c>
-      <c r="C196" s="5" t="s">
-        <v>1199</v>
       </c>
       <c r="D196" s="6"/>
       <c r="E196" s="6"/>
@@ -12752,13 +12754,13 @@
     </row>
     <row r="197" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A197" s="12" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B197" s="5" t="s">
         <v>1200</v>
       </c>
-      <c r="B197" s="5" t="s">
+      <c r="C197" s="5" t="s">
         <v>1201</v>
-      </c>
-      <c r="C197" s="5" t="s">
-        <v>1202</v>
       </c>
       <c r="D197" s="6"/>
       <c r="E197" s="6"/>
@@ -12786,13 +12788,13 @@
     </row>
     <row r="198" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A198" s="12" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B198" s="5" t="s">
         <v>1203</v>
       </c>
-      <c r="B198" s="5" t="s">
+      <c r="C198" s="5" t="s">
         <v>1204</v>
-      </c>
-      <c r="C198" s="5" t="s">
-        <v>1205</v>
       </c>
       <c r="D198" s="6"/>
       <c r="E198" s="6"/>
@@ -12820,13 +12822,13 @@
     </row>
     <row r="199" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A199" s="12" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B199" s="5" t="s">
         <v>1206</v>
       </c>
-      <c r="B199" s="5" t="s">
+      <c r="C199" s="5" t="s">
         <v>1207</v>
-      </c>
-      <c r="C199" s="5" t="s">
-        <v>1208</v>
       </c>
       <c r="D199" s="6"/>
       <c r="E199" s="6"/>
@@ -12854,13 +12856,13 @@
     </row>
     <row r="200" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A200" s="12" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B200" s="5" t="s">
         <v>1209</v>
       </c>
-      <c r="B200" s="5" t="s">
+      <c r="C200" s="5" t="s">
         <v>1210</v>
-      </c>
-      <c r="C200" s="5" t="s">
-        <v>1211</v>
       </c>
       <c r="D200" s="6"/>
       <c r="E200" s="6"/>
@@ -12888,13 +12890,13 @@
     </row>
     <row r="201" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A201" s="12" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B201" s="5" t="s">
         <v>1212</v>
       </c>
-      <c r="B201" s="5" t="s">
+      <c r="C201" s="5" t="s">
         <v>1213</v>
-      </c>
-      <c r="C201" s="5" t="s">
-        <v>1214</v>
       </c>
       <c r="D201" s="6"/>
       <c r="E201" s="6"/>
@@ -12956,13 +12958,13 @@
     </row>
     <row r="203" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A203" s="12" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B203" s="5" t="s">
         <v>1215</v>
       </c>
-      <c r="B203" s="5" t="s">
+      <c r="C203" s="5" t="s">
         <v>1216</v>
-      </c>
-      <c r="C203" s="5" t="s">
-        <v>1217</v>
       </c>
       <c r="D203" s="6"/>
       <c r="E203" s="6"/>
@@ -12990,13 +12992,13 @@
     </row>
     <row r="204" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A204" s="12" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B204" s="5" t="s">
         <v>1218</v>
       </c>
-      <c r="B204" s="5" t="s">
+      <c r="C204" s="5" t="s">
         <v>1219</v>
-      </c>
-      <c r="C204" s="5" t="s">
-        <v>1220</v>
       </c>
       <c r="D204" s="6"/>
       <c r="E204" s="6"/>
@@ -13024,13 +13026,13 @@
     </row>
     <row r="205" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A205" s="12" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B205" s="5" t="s">
         <v>1221</v>
       </c>
-      <c r="B205" s="5" t="s">
+      <c r="C205" s="5" t="s">
         <v>1222</v>
-      </c>
-      <c r="C205" s="5" t="s">
-        <v>1223</v>
       </c>
       <c r="D205" s="6"/>
       <c r="E205" s="6"/>
@@ -13228,13 +13230,13 @@
     </row>
     <row r="211" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A211" s="12" t="s">
+        <v>1223</v>
+      </c>
+      <c r="B211" s="5" t="s">
         <v>1224</v>
       </c>
-      <c r="B211" s="5" t="s">
+      <c r="C211" s="5" t="s">
         <v>1225</v>
-      </c>
-      <c r="C211" s="5" t="s">
-        <v>1226</v>
       </c>
       <c r="D211" s="6"/>
       <c r="E211" s="6"/>
@@ -13568,13 +13570,13 @@
     </row>
     <row r="221" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A221" s="12" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B221" s="5" t="s">
         <v>1227</v>
       </c>
-      <c r="B221" s="5" t="s">
+      <c r="C221" s="5" t="s">
         <v>1228</v>
-      </c>
-      <c r="C221" s="5" t="s">
-        <v>1229</v>
       </c>
       <c r="D221" s="6"/>
       <c r="E221" s="6"/>
@@ -13840,13 +13842,13 @@
     </row>
     <row r="229" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A229" s="12" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B229" s="5" t="s">
         <v>1230</v>
       </c>
-      <c r="B229" s="5" t="s">
+      <c r="C229" s="5" t="s">
         <v>1231</v>
-      </c>
-      <c r="C229" s="5" t="s">
-        <v>1232</v>
       </c>
       <c r="D229" s="6"/>
       <c r="E229" s="6"/>
@@ -13874,13 +13876,13 @@
     </row>
     <row r="230" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A230" s="12" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B230" s="5" t="s">
         <v>1233</v>
       </c>
-      <c r="B230" s="5" t="s">
+      <c r="C230" s="5" t="s">
         <v>1234</v>
-      </c>
-      <c r="C230" s="5" t="s">
-        <v>1235</v>
       </c>
       <c r="D230" s="6"/>
       <c r="E230" s="6"/>
@@ -13911,10 +13913,10 @@
         <v>57</v>
       </c>
       <c r="B231" s="5" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C231" s="5" t="s">
         <v>1236</v>
-      </c>
-      <c r="C231" s="5" t="s">
-        <v>1237</v>
       </c>
       <c r="D231" s="6"/>
       <c r="E231" s="6"/>
@@ -13942,13 +13944,13 @@
     </row>
     <row r="232" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A232" s="12" t="s">
+        <v>1237</v>
+      </c>
+      <c r="B232" s="5" t="s">
         <v>1238</v>
       </c>
-      <c r="B232" s="5" t="s">
+      <c r="C232" s="5" t="s">
         <v>1239</v>
-      </c>
-      <c r="C232" s="5" t="s">
-        <v>1240</v>
       </c>
       <c r="D232" s="6"/>
       <c r="E232" s="6"/>
@@ -13976,13 +13978,13 @@
     </row>
     <row r="233" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A233" s="12" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B233" s="5" t="s">
         <v>1241</v>
       </c>
-      <c r="B233" s="5" t="s">
+      <c r="C233" s="5" t="s">
         <v>1242</v>
-      </c>
-      <c r="C233" s="5" t="s">
-        <v>1243</v>
       </c>
       <c r="D233" s="6"/>
       <c r="E233" s="6"/>
@@ -14248,13 +14250,13 @@
     </row>
     <row r="241" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A241" s="12" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B241" s="5" t="s">
         <v>1244</v>
       </c>
-      <c r="B241" s="5" t="s">
+      <c r="C241" s="5" t="s">
         <v>1245</v>
-      </c>
-      <c r="C241" s="5" t="s">
-        <v>1246</v>
       </c>
       <c r="D241" s="6"/>
       <c r="E241" s="6"/>
@@ -14316,13 +14318,13 @@
     </row>
     <row r="243" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A243" s="12" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B243" s="5" t="s">
         <v>1247</v>
       </c>
-      <c r="B243" s="5" t="s">
+      <c r="C243" s="5" t="s">
         <v>1248</v>
-      </c>
-      <c r="C243" s="5" t="s">
-        <v>1249</v>
       </c>
       <c r="D243" s="6"/>
       <c r="E243" s="6"/>
@@ -14384,13 +14386,13 @@
     </row>
     <row r="245" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A245" s="12" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B245" s="5" t="s">
         <v>1250</v>
       </c>
-      <c r="B245" s="5" t="s">
+      <c r="C245" s="5" t="s">
         <v>1251</v>
-      </c>
-      <c r="C245" s="5" t="s">
-        <v>1252</v>
       </c>
       <c r="D245" s="6"/>
       <c r="E245" s="6"/>
@@ -14554,13 +14556,13 @@
     </row>
     <row r="250" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A250" s="12" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B250" s="5" t="s">
         <v>1253</v>
       </c>
-      <c r="B250" s="5" t="s">
+      <c r="C250" s="5" t="s">
         <v>1254</v>
-      </c>
-      <c r="C250" s="5" t="s">
-        <v>1255</v>
       </c>
       <c r="D250" s="6"/>
       <c r="E250" s="6"/>
@@ -14588,13 +14590,13 @@
     </row>
     <row r="251" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A251" s="12" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B251" s="5" t="s">
         <v>1256</v>
       </c>
-      <c r="B251" s="5" t="s">
+      <c r="C251" s="5" t="s">
         <v>1257</v>
-      </c>
-      <c r="C251" s="5" t="s">
-        <v>1258</v>
       </c>
       <c r="D251" s="6"/>
       <c r="E251" s="6"/>
@@ -14622,13 +14624,13 @@
     </row>
     <row r="252" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A252" s="12" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B252" s="5" t="s">
         <v>1259</v>
       </c>
-      <c r="B252" s="5" t="s">
+      <c r="C252" s="5" t="s">
         <v>1260</v>
-      </c>
-      <c r="C252" s="5" t="s">
-        <v>1261</v>
       </c>
       <c r="D252" s="6"/>
       <c r="E252" s="6"/>
@@ -14656,13 +14658,13 @@
     </row>
     <row r="253" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A253" s="12" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B253" s="7" t="s">
         <v>1262</v>
       </c>
-      <c r="B253" s="7" t="s">
+      <c r="C253" s="5" t="s">
         <v>1263</v>
-      </c>
-      <c r="C253" s="5" t="s">
-        <v>1264</v>
       </c>
       <c r="D253" s="6"/>
       <c r="E253" s="6"/>
@@ -14690,13 +14692,13 @@
     </row>
     <row r="254" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A254" s="12" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B254" s="7" t="s">
         <v>1265</v>
       </c>
-      <c r="B254" s="7" t="s">
+      <c r="C254" s="5" t="s">
         <v>1266</v>
-      </c>
-      <c r="C254" s="5" t="s">
-        <v>1267</v>
       </c>
       <c r="D254" s="6"/>
       <c r="E254" s="6"/>
@@ -14724,13 +14726,13 @@
     </row>
     <row r="255" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A255" s="12" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B255" s="7" t="s">
         <v>1268</v>
       </c>
-      <c r="B255" s="7" t="s">
+      <c r="C255" s="5" t="s">
         <v>1269</v>
-      </c>
-      <c r="C255" s="5" t="s">
-        <v>1270</v>
       </c>
       <c r="D255" s="6"/>
       <c r="E255" s="6"/>
@@ -14758,13 +14760,13 @@
     </row>
     <row r="256" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A256" s="12" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B256" s="7" t="s">
         <v>1271</v>
       </c>
-      <c r="B256" s="7" t="s">
+      <c r="C256" s="5" t="s">
         <v>1272</v>
-      </c>
-      <c r="C256" s="5" t="s">
-        <v>1273</v>
       </c>
       <c r="D256" s="6"/>
       <c r="E256" s="6"/>
@@ -14792,13 +14794,13 @@
     </row>
     <row r="257" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A257" s="12" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B257" s="7" t="s">
         <v>1274</v>
       </c>
-      <c r="B257" s="7" t="s">
+      <c r="C257" s="5" t="s">
         <v>1275</v>
-      </c>
-      <c r="C257" s="5" t="s">
-        <v>1276</v>
       </c>
       <c r="D257" s="6"/>
       <c r="E257" s="6"/>
@@ -14826,13 +14828,13 @@
     </row>
     <row r="258" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A258" s="12" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B258" s="5" t="s">
         <v>1277</v>
       </c>
-      <c r="B258" s="5" t="s">
+      <c r="C258" s="5" t="s">
         <v>1278</v>
-      </c>
-      <c r="C258" s="5" t="s">
-        <v>1279</v>
       </c>
       <c r="D258" s="6"/>
       <c r="E258" s="6"/>
@@ -14860,13 +14862,13 @@
     </row>
     <row r="259" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A259" s="12" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B259" s="5" t="s">
         <v>1280</v>
       </c>
-      <c r="B259" s="5" t="s">
+      <c r="C259" s="8" t="s">
         <v>1281</v>
-      </c>
-      <c r="C259" s="8" t="s">
-        <v>1282</v>
       </c>
       <c r="D259" s="6"/>
       <c r="E259" s="6"/>
@@ -15030,13 +15032,13 @@
     </row>
     <row r="264" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A264" s="12" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B264" s="6" t="s">
         <v>1283</v>
       </c>
-      <c r="B264" s="6" t="s">
+      <c r="C264" s="6" t="s">
         <v>1284</v>
-      </c>
-      <c r="C264" s="6" t="s">
-        <v>1285</v>
       </c>
       <c r="D264" s="6"/>
       <c r="E264" s="6"/>
@@ -15064,13 +15066,13 @@
     </row>
     <row r="265" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A265" s="12" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B265" s="6" t="s">
         <v>1286</v>
       </c>
-      <c r="B265" s="6" t="s">
+      <c r="C265" s="6" t="s">
         <v>1287</v>
-      </c>
-      <c r="C265" s="6" t="s">
-        <v>1288</v>
       </c>
       <c r="D265" s="6"/>
       <c r="E265" s="6"/>
@@ -15234,13 +15236,13 @@
     </row>
     <row r="270" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A270" s="12" t="s">
+        <v>1288</v>
+      </c>
+      <c r="B270" s="6" t="s">
         <v>1289</v>
       </c>
-      <c r="B270" s="6" t="s">
+      <c r="C270" s="6" t="s">
         <v>1290</v>
-      </c>
-      <c r="C270" s="6" t="s">
-        <v>1291</v>
       </c>
       <c r="D270" s="6"/>
       <c r="E270" s="6"/>
@@ -15268,13 +15270,13 @@
     </row>
     <row r="271" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A271" s="12" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B271" s="6" t="s">
         <v>1292</v>
       </c>
-      <c r="B271" s="6" t="s">
+      <c r="C271" s="6" t="s">
         <v>1293</v>
-      </c>
-      <c r="C271" s="6" t="s">
-        <v>1294</v>
       </c>
       <c r="D271" s="6"/>
       <c r="E271" s="6"/>
@@ -15336,13 +15338,13 @@
     </row>
     <row r="273" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A273" s="12" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B273" s="6" t="s">
         <v>1295</v>
       </c>
-      <c r="B273" s="6" t="s">
+      <c r="C273" s="6" t="s">
         <v>1296</v>
-      </c>
-      <c r="C273" s="6" t="s">
-        <v>1297</v>
       </c>
       <c r="D273" s="6"/>
       <c r="E273" s="6"/>
@@ -15370,13 +15372,13 @@
     </row>
     <row r="274" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A274" s="12" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B274" s="6" t="s">
         <v>1298</v>
       </c>
-      <c r="B274" s="6" t="s">
+      <c r="C274" s="6" t="s">
         <v>1299</v>
-      </c>
-      <c r="C274" s="6" t="s">
-        <v>1300</v>
       </c>
       <c r="D274" s="6"/>
       <c r="E274" s="6"/>
@@ -15404,13 +15406,13 @@
     </row>
     <row r="275" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A275" s="12" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B275" s="6" t="s">
         <v>1301</v>
       </c>
-      <c r="B275" s="6" t="s">
+      <c r="C275" s="6" t="s">
         <v>1302</v>
-      </c>
-      <c r="C275" s="6" t="s">
-        <v>1303</v>
       </c>
       <c r="D275" s="6"/>
       <c r="E275" s="6"/>
@@ -15506,13 +15508,13 @@
     </row>
     <row r="278" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A278" s="12" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B278" s="6" t="s">
         <v>1304</v>
       </c>
-      <c r="B278" s="6" t="s">
+      <c r="C278" s="6" t="s">
         <v>1305</v>
-      </c>
-      <c r="C278" s="6" t="s">
-        <v>1306</v>
       </c>
       <c r="D278" s="6"/>
       <c r="E278" s="6"/>
@@ -15642,13 +15644,13 @@
     </row>
     <row r="282" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A282" s="12" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B282" s="6" t="s">
         <v>1307</v>
       </c>
-      <c r="B282" s="6" t="s">
+      <c r="C282" s="6" t="s">
         <v>1308</v>
-      </c>
-      <c r="C282" s="6" t="s">
-        <v>1309</v>
       </c>
       <c r="D282" s="6"/>
       <c r="E282" s="6"/>
@@ -15676,13 +15678,13 @@
     </row>
     <row r="283" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A283" s="12" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B283" s="6" t="s">
         <v>1310</v>
       </c>
-      <c r="B283" s="6" t="s">
+      <c r="C283" s="6" t="s">
         <v>1311</v>
-      </c>
-      <c r="C283" s="6" t="s">
-        <v>1312</v>
       </c>
       <c r="D283" s="6"/>
       <c r="E283" s="6"/>
@@ -15710,13 +15712,13 @@
     </row>
     <row r="284" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A284" s="12" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B284" s="6" t="s">
         <v>1313</v>
       </c>
-      <c r="B284" s="6" t="s">
+      <c r="C284" s="6" t="s">
         <v>1314</v>
-      </c>
-      <c r="C284" s="6" t="s">
-        <v>1315</v>
       </c>
       <c r="D284" s="6"/>
       <c r="E284" s="6"/>
@@ -15880,13 +15882,13 @@
     </row>
     <row r="289" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A289" s="12" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B289" s="6" t="s">
         <v>1316</v>
       </c>
-      <c r="B289" s="6" t="s">
+      <c r="C289" s="6" t="s">
         <v>1317</v>
-      </c>
-      <c r="C289" s="6" t="s">
-        <v>1318</v>
       </c>
       <c r="D289" s="6"/>
       <c r="E289" s="6"/>
@@ -15914,13 +15916,13 @@
     </row>
     <row r="290" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A290" s="12" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B290" s="6" t="s">
         <v>1319</v>
       </c>
-      <c r="B290" s="6" t="s">
+      <c r="C290" s="6" t="s">
         <v>1320</v>
-      </c>
-      <c r="C290" s="6" t="s">
-        <v>1321</v>
       </c>
       <c r="D290" s="6"/>
       <c r="E290" s="6"/>
@@ -15948,13 +15950,13 @@
     </row>
     <row r="291" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A291" s="12" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B291" s="6" t="s">
         <v>1322</v>
       </c>
-      <c r="B291" s="6" t="s">
+      <c r="C291" s="6" t="s">
         <v>1323</v>
-      </c>
-      <c r="C291" s="6" t="s">
-        <v>1324</v>
       </c>
       <c r="D291" s="6"/>
       <c r="E291" s="6"/>
@@ -15982,13 +15984,13 @@
     </row>
     <row r="292" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A292" s="12" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B292" s="6" t="s">
         <v>1325</v>
       </c>
-      <c r="B292" s="6" t="s">
+      <c r="C292" s="6" t="s">
         <v>1326</v>
-      </c>
-      <c r="C292" s="6" t="s">
-        <v>1327</v>
       </c>
       <c r="D292" s="6"/>
       <c r="E292" s="6"/>
@@ -16016,13 +16018,13 @@
     </row>
     <row r="293" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A293" s="12" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B293" s="6" t="s">
         <v>1328</v>
       </c>
-      <c r="B293" s="6" t="s">
+      <c r="C293" s="6" t="s">
         <v>1329</v>
-      </c>
-      <c r="C293" s="6" t="s">
-        <v>1330</v>
       </c>
       <c r="D293" s="6"/>
       <c r="E293" s="6"/>
@@ -16084,13 +16086,13 @@
     </row>
     <row r="295" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A295" s="12" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B295" s="6" t="s">
         <v>1331</v>
       </c>
-      <c r="B295" s="6" t="s">
+      <c r="C295" s="6" t="s">
         <v>1332</v>
-      </c>
-      <c r="C295" s="6" t="s">
-        <v>1333</v>
       </c>
       <c r="D295" s="6"/>
       <c r="E295" s="6"/>
@@ -16186,13 +16188,13 @@
     </row>
     <row r="298" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A298" s="12" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B298" s="6" t="s">
         <v>1334</v>
       </c>
-      <c r="B298" s="6" t="s">
+      <c r="C298" s="6" t="s">
         <v>1335</v>
-      </c>
-      <c r="C298" s="6" t="s">
-        <v>1336</v>
       </c>
       <c r="D298" s="6"/>
       <c r="E298" s="6"/>
@@ -16220,13 +16222,13 @@
     </row>
     <row r="299" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A299" s="12" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B299" s="6" t="s">
         <v>1337</v>
       </c>
-      <c r="B299" s="6" t="s">
+      <c r="C299" s="6" t="s">
         <v>1338</v>
-      </c>
-      <c r="C299" s="6" t="s">
-        <v>1339</v>
       </c>
       <c r="D299" s="6"/>
       <c r="E299" s="6"/>
@@ -16254,13 +16256,13 @@
     </row>
     <row r="300" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A300" s="12" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B300" s="6" t="s">
         <v>1340</v>
       </c>
-      <c r="B300" s="6" t="s">
+      <c r="C300" s="6" t="s">
         <v>1341</v>
-      </c>
-      <c r="C300" s="6" t="s">
-        <v>1342</v>
       </c>
       <c r="D300" s="6"/>
       <c r="E300" s="6"/>
@@ -16288,13 +16290,13 @@
     </row>
     <row r="301" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A301" s="12" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B301" s="6" t="s">
         <v>1343</v>
       </c>
-      <c r="B301" s="6" t="s">
+      <c r="C301" s="6" t="s">
         <v>1344</v>
-      </c>
-      <c r="C301" s="6" t="s">
-        <v>1345</v>
       </c>
       <c r="D301" s="6"/>
       <c r="E301" s="6"/>
@@ -16492,13 +16494,13 @@
     </row>
     <row r="307" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A307" s="12" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B307" s="6" t="s">
         <v>1346</v>
       </c>
-      <c r="B307" s="6" t="s">
+      <c r="C307" s="6" t="s">
         <v>1347</v>
-      </c>
-      <c r="C307" s="6" t="s">
-        <v>1348</v>
       </c>
       <c r="D307" s="6"/>
       <c r="E307" s="6"/>
@@ -16560,13 +16562,13 @@
     </row>
     <row r="309" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A309" s="12" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B309" s="6" t="s">
         <v>1349</v>
       </c>
-      <c r="B309" s="6" t="s">
+      <c r="C309" s="6" t="s">
         <v>1350</v>
-      </c>
-      <c r="C309" s="6" t="s">
-        <v>1351</v>
       </c>
       <c r="D309" s="6"/>
       <c r="E309" s="6"/>
@@ -17002,13 +17004,13 @@
     </row>
     <row r="322" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A322" s="12" t="s">
+        <v>1351</v>
+      </c>
+      <c r="B322" s="6" t="s">
         <v>1352</v>
       </c>
-      <c r="B322" s="6" t="s">
+      <c r="C322" s="6" t="s">
         <v>1353</v>
-      </c>
-      <c r="C322" s="6" t="s">
-        <v>1354</v>
       </c>
       <c r="D322" s="6"/>
       <c r="E322" s="6"/>
@@ -17036,13 +17038,13 @@
     </row>
     <row r="323" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A323" s="12" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B323" s="6" t="s">
         <v>1355</v>
       </c>
-      <c r="B323" s="6" t="s">
+      <c r="C323" s="6" t="s">
         <v>1356</v>
-      </c>
-      <c r="C323" s="6" t="s">
-        <v>1357</v>
       </c>
       <c r="D323" s="6"/>
       <c r="E323" s="6"/>
@@ -17070,13 +17072,13 @@
     </row>
     <row r="324" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A324" s="12" t="s">
+        <v>1357</v>
+      </c>
+      <c r="B324" s="6" t="s">
         <v>1358</v>
       </c>
-      <c r="B324" s="6" t="s">
+      <c r="C324" s="6" t="s">
         <v>1359</v>
-      </c>
-      <c r="C324" s="6" t="s">
-        <v>1360</v>
       </c>
       <c r="D324" s="6"/>
       <c r="E324" s="6"/>
@@ -17342,13 +17344,13 @@
     </row>
     <row r="332" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A332" s="12" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B332" s="6" t="s">
         <v>1361</v>
       </c>
-      <c r="B332" s="6" t="s">
+      <c r="C332" s="6" t="s">
         <v>1362</v>
-      </c>
-      <c r="C332" s="6" t="s">
-        <v>1363</v>
       </c>
       <c r="D332" s="6"/>
       <c r="E332" s="6"/>
@@ -17376,13 +17378,13 @@
     </row>
     <row r="333" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A333" s="12" t="s">
+        <v>1363</v>
+      </c>
+      <c r="B333" s="6" t="s">
         <v>1364</v>
       </c>
-      <c r="B333" s="6" t="s">
+      <c r="C333" s="6" t="s">
         <v>1365</v>
-      </c>
-      <c r="C333" s="6" t="s">
-        <v>1366</v>
       </c>
       <c r="D333" s="6"/>
       <c r="E333" s="6"/>
@@ -17444,13 +17446,13 @@
     </row>
     <row r="335" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A335" s="12" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B335" s="6" t="s">
         <v>1367</v>
       </c>
-      <c r="B335" s="6" t="s">
+      <c r="C335" s="6" t="s">
         <v>1368</v>
-      </c>
-      <c r="C335" s="6" t="s">
-        <v>1369</v>
       </c>
       <c r="D335" s="6"/>
       <c r="E335" s="6"/>
@@ -17478,13 +17480,13 @@
     </row>
     <row r="336" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A336" s="12" t="s">
+        <v>1369</v>
+      </c>
+      <c r="B336" s="6" t="s">
         <v>1370</v>
       </c>
-      <c r="B336" s="6" t="s">
+      <c r="C336" s="6" t="s">
         <v>1371</v>
-      </c>
-      <c r="C336" s="6" t="s">
-        <v>1372</v>
       </c>
       <c r="D336" s="6"/>
       <c r="E336" s="6"/>
@@ -17546,13 +17548,13 @@
     </row>
     <row r="338" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A338" s="12" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B338" s="6" t="s">
         <v>1373</v>
       </c>
-      <c r="B338" s="6" t="s">
+      <c r="C338" s="6" t="s">
         <v>1374</v>
-      </c>
-      <c r="C338" s="6" t="s">
-        <v>1375</v>
       </c>
       <c r="D338" s="6"/>
       <c r="E338" s="6"/>
@@ -17580,13 +17582,13 @@
     </row>
     <row r="339" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A339" s="12" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B339" s="6" t="s">
         <v>1376</v>
       </c>
-      <c r="B339" s="6" t="s">
+      <c r="C339" s="6" t="s">
         <v>1377</v>
-      </c>
-      <c r="C339" s="6" t="s">
-        <v>1378</v>
       </c>
       <c r="D339" s="6"/>
       <c r="E339" s="6"/>
@@ -17614,13 +17616,13 @@
     </row>
     <row r="340" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A340" s="12" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B340" s="6" t="s">
         <v>1379</v>
       </c>
-      <c r="B340" s="6" t="s">
+      <c r="C340" s="6" t="s">
         <v>1380</v>
-      </c>
-      <c r="C340" s="6" t="s">
-        <v>1381</v>
       </c>
       <c r="D340" s="6"/>
       <c r="E340" s="6"/>
@@ -17648,13 +17650,13 @@
     </row>
     <row r="341" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A341" s="12" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B341" s="6" t="s">
         <v>1382</v>
       </c>
-      <c r="B341" s="6" t="s">
+      <c r="C341" s="6" t="s">
         <v>1383</v>
-      </c>
-      <c r="C341" s="6" t="s">
-        <v>1384</v>
       </c>
       <c r="D341" s="6"/>
       <c r="E341" s="6"/>
@@ -17682,13 +17684,13 @@
     </row>
     <row r="342" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A342" s="12" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B342" s="6" t="s">
         <v>1385</v>
       </c>
-      <c r="B342" s="6" t="s">
+      <c r="C342" s="6" t="s">
         <v>1386</v>
-      </c>
-      <c r="C342" s="6" t="s">
-        <v>1387</v>
       </c>
       <c r="D342" s="6"/>
       <c r="E342" s="6"/>
@@ -17716,13 +17718,13 @@
     </row>
     <row r="343" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A343" s="12" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B343" s="6" t="s">
         <v>1388</v>
       </c>
-      <c r="B343" s="6" t="s">
+      <c r="C343" s="6" t="s">
         <v>1389</v>
-      </c>
-      <c r="C343" s="6" t="s">
-        <v>1390</v>
       </c>
       <c r="D343" s="6"/>
       <c r="E343" s="6"/>
@@ -17750,13 +17752,13 @@
     </row>
     <row r="344" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A344" s="12" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B344" s="6" t="s">
         <v>1391</v>
       </c>
-      <c r="B344" s="6" t="s">
+      <c r="C344" s="6" t="s">
         <v>1392</v>
-      </c>
-      <c r="C344" s="6" t="s">
-        <v>1393</v>
       </c>
       <c r="D344" s="6"/>
       <c r="E344" s="6"/>
@@ -17784,13 +17786,13 @@
     </row>
     <row r="345" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A345" s="12" t="s">
+        <v>1393</v>
+      </c>
+      <c r="B345" s="6" t="s">
         <v>1394</v>
       </c>
-      <c r="B345" s="6" t="s">
+      <c r="C345" s="6" t="s">
         <v>1395</v>
-      </c>
-      <c r="C345" s="6" t="s">
-        <v>1396</v>
       </c>
       <c r="D345" s="6"/>
       <c r="E345" s="6"/>
@@ -17818,13 +17820,13 @@
     </row>
     <row r="346" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A346" s="12" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B346" s="6" t="s">
         <v>1397</v>
       </c>
-      <c r="B346" s="6" t="s">
+      <c r="C346" s="6" t="s">
         <v>1398</v>
-      </c>
-      <c r="C346" s="6" t="s">
-        <v>1399</v>
       </c>
       <c r="D346" s="6"/>
       <c r="E346" s="6"/>
@@ -17852,13 +17854,13 @@
     </row>
     <row r="347" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A347" s="12" t="s">
+        <v>1399</v>
+      </c>
+      <c r="B347" s="6" t="s">
         <v>1400</v>
       </c>
-      <c r="B347" s="6" t="s">
+      <c r="C347" s="6" t="s">
         <v>1401</v>
-      </c>
-      <c r="C347" s="6" t="s">
-        <v>1402</v>
       </c>
       <c r="D347" s="6"/>
       <c r="E347" s="6"/>
@@ -17920,13 +17922,13 @@
     </row>
     <row r="349" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A349" s="12" t="s">
+        <v>1402</v>
+      </c>
+      <c r="B349" s="6" t="s">
         <v>1403</v>
       </c>
-      <c r="B349" s="6" t="s">
+      <c r="C349" s="6" t="s">
         <v>1404</v>
-      </c>
-      <c r="C349" s="6" t="s">
-        <v>1405</v>
       </c>
       <c r="D349" s="6"/>
       <c r="E349" s="6"/>
@@ -18022,13 +18024,13 @@
     </row>
     <row r="352" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A352" s="12" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B352" s="6" t="s">
         <v>1406</v>
       </c>
-      <c r="B352" s="6" t="s">
+      <c r="C352" s="6" t="s">
         <v>1407</v>
-      </c>
-      <c r="C352" s="6" t="s">
-        <v>1408</v>
       </c>
       <c r="D352" s="6"/>
       <c r="E352" s="6"/>
@@ -18158,13 +18160,13 @@
     </row>
     <row r="356" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A356" s="12" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B356" s="6" t="s">
         <v>1409</v>
       </c>
-      <c r="B356" s="6" t="s">
+      <c r="C356" s="6" t="s">
         <v>1410</v>
-      </c>
-      <c r="C356" s="6" t="s">
-        <v>1411</v>
       </c>
       <c r="D356" s="6"/>
       <c r="E356" s="6"/>
@@ -18192,13 +18194,13 @@
     </row>
     <row r="357" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A357" s="12" t="s">
+        <v>1411</v>
+      </c>
+      <c r="B357" s="6" t="s">
         <v>1412</v>
       </c>
-      <c r="B357" s="6" t="s">
+      <c r="C357" s="6" t="s">
         <v>1413</v>
-      </c>
-      <c r="C357" s="6" t="s">
-        <v>1414</v>
       </c>
       <c r="D357" s="6"/>
       <c r="E357" s="6"/>
@@ -18226,13 +18228,13 @@
     </row>
     <row r="358" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A358" s="12" t="s">
+        <v>1414</v>
+      </c>
+      <c r="B358" s="6" t="s">
         <v>1415</v>
       </c>
-      <c r="B358" s="6" t="s">
+      <c r="C358" s="6" t="s">
         <v>1416</v>
-      </c>
-      <c r="C358" s="6" t="s">
-        <v>1417</v>
       </c>
       <c r="D358" s="6"/>
       <c r="E358" s="6"/>
@@ -18260,13 +18262,13 @@
     </row>
     <row r="359" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A359" s="12" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B359" s="6" t="s">
         <v>1418</v>
       </c>
-      <c r="B359" s="6" t="s">
+      <c r="C359" s="6" t="s">
         <v>1419</v>
-      </c>
-      <c r="C359" s="6" t="s">
-        <v>1420</v>
       </c>
       <c r="D359" s="6"/>
       <c r="E359" s="6"/>
@@ -18328,13 +18330,13 @@
     </row>
     <row r="361" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A361" s="12" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B361" s="6" t="s">
         <v>1421</v>
       </c>
-      <c r="B361" s="6" t="s">
+      <c r="C361" s="6" t="s">
         <v>1422</v>
-      </c>
-      <c r="C361" s="6" t="s">
-        <v>1423</v>
       </c>
       <c r="D361" s="6"/>
       <c r="E361" s="6"/>
@@ -18566,13 +18568,13 @@
     </row>
     <row r="368" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A368" s="12" t="s">
+        <v>1423</v>
+      </c>
+      <c r="B368" s="6" t="s">
         <v>1424</v>
       </c>
-      <c r="B368" s="6" t="s">
+      <c r="C368" s="6" t="s">
         <v>1425</v>
-      </c>
-      <c r="C368" s="6" t="s">
-        <v>1426</v>
       </c>
       <c r="D368" s="6"/>
       <c r="E368" s="6"/>
@@ -18702,13 +18704,13 @@
     </row>
     <row r="372" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A372" s="12" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B372" s="6" t="s">
         <v>1427</v>
       </c>
-      <c r="B372" s="6" t="s">
+      <c r="C372" s="6" t="s">
         <v>1428</v>
-      </c>
-      <c r="C372" s="6" t="s">
-        <v>1429</v>
       </c>
       <c r="D372" s="6"/>
       <c r="E372" s="6"/>
@@ -18770,13 +18772,13 @@
     </row>
     <row r="374" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A374" s="12" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B374" s="6" t="s">
         <v>1430</v>
       </c>
-      <c r="B374" s="6" t="s">
+      <c r="C374" s="6" t="s">
         <v>1431</v>
-      </c>
-      <c r="C374" s="6" t="s">
-        <v>1432</v>
       </c>
       <c r="D374" s="6"/>
       <c r="E374" s="6"/>
@@ -19212,13 +19214,13 @@
     </row>
     <row r="387" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A387" s="12" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B387" s="6" t="s">
         <v>1433</v>
       </c>
-      <c r="B387" s="6" t="s">
+      <c r="C387" s="6" t="s">
         <v>1434</v>
-      </c>
-      <c r="C387" s="6" t="s">
-        <v>1435</v>
       </c>
       <c r="D387" s="6"/>
       <c r="E387" s="6"/>
@@ -19246,13 +19248,13 @@
     </row>
     <row r="388" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A388" s="12" t="s">
+        <v>1435</v>
+      </c>
+      <c r="B388" s="6" t="s">
         <v>1436</v>
       </c>
-      <c r="B388" s="6" t="s">
+      <c r="C388" s="6" t="s">
         <v>1437</v>
-      </c>
-      <c r="C388" s="6" t="s">
-        <v>1438</v>
       </c>
       <c r="D388" s="6"/>
       <c r="E388" s="6"/>
@@ -19552,13 +19554,13 @@
     </row>
     <row r="397" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A397" s="12" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B397" s="6" t="s">
         <v>1439</v>
       </c>
-      <c r="B397" s="6" t="s">
+      <c r="C397" s="6" t="s">
         <v>1440</v>
-      </c>
-      <c r="C397" s="6" t="s">
-        <v>1441</v>
       </c>
       <c r="D397" s="6"/>
       <c r="E397" s="6"/>
@@ -19586,13 +19588,13 @@
     </row>
     <row r="398" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A398" s="12" t="s">
+        <v>1441</v>
+      </c>
+      <c r="B398" s="6" t="s">
         <v>1442</v>
       </c>
-      <c r="B398" s="6" t="s">
+      <c r="C398" s="6" t="s">
         <v>1443</v>
-      </c>
-      <c r="C398" s="6" t="s">
-        <v>1444</v>
       </c>
       <c r="D398" s="6"/>
       <c r="E398" s="6"/>
@@ -19620,13 +19622,13 @@
     </row>
     <row r="399" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A399" s="12" t="s">
+        <v>1444</v>
+      </c>
+      <c r="B399" s="6" t="s">
         <v>1445</v>
       </c>
-      <c r="B399" s="6" t="s">
+      <c r="C399" s="6" t="s">
         <v>1446</v>
-      </c>
-      <c r="C399" s="6" t="s">
-        <v>1447</v>
       </c>
       <c r="D399" s="6"/>
       <c r="E399" s="6"/>
@@ -19654,13 +19656,13 @@
     </row>
     <row r="400" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A400" s="12" t="s">
+        <v>1447</v>
+      </c>
+      <c r="B400" s="6" t="s">
         <v>1448</v>
       </c>
-      <c r="B400" s="6" t="s">
+      <c r="C400" s="6" t="s">
         <v>1449</v>
-      </c>
-      <c r="C400" s="6" t="s">
-        <v>1450</v>
       </c>
       <c r="D400" s="6"/>
       <c r="E400" s="6"/>
@@ -19688,13 +19690,13 @@
     </row>
     <row r="401" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A401" s="12" t="s">
+        <v>1450</v>
+      </c>
+      <c r="B401" s="6" t="s">
         <v>1451</v>
       </c>
-      <c r="B401" s="6" t="s">
+      <c r="C401" s="6" t="s">
         <v>1452</v>
-      </c>
-      <c r="C401" s="6" t="s">
-        <v>1453</v>
       </c>
       <c r="D401" s="6"/>
       <c r="E401" s="6"/>
@@ -19722,13 +19724,13 @@
     </row>
     <row r="402" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A402" s="12" t="s">
+        <v>1453</v>
+      </c>
+      <c r="B402" s="6" t="s">
         <v>1454</v>
       </c>
-      <c r="B402" s="6" t="s">
+      <c r="C402" s="6" t="s">
         <v>1455</v>
-      </c>
-      <c r="C402" s="6" t="s">
-        <v>1456</v>
       </c>
       <c r="D402" s="6"/>
       <c r="E402" s="6"/>
@@ -19756,13 +19758,13 @@
     </row>
     <row r="403" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A403" s="12" t="s">
+        <v>1456</v>
+      </c>
+      <c r="B403" s="6" t="s">
         <v>1457</v>
       </c>
-      <c r="B403" s="6" t="s">
+      <c r="C403" s="6" t="s">
         <v>1458</v>
-      </c>
-      <c r="C403" s="6" t="s">
-        <v>1459</v>
       </c>
       <c r="D403" s="6"/>
       <c r="E403" s="6"/>
@@ -19790,13 +19792,13 @@
     </row>
     <row r="404" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A404" s="12" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B404" s="6" t="s">
         <v>1460</v>
       </c>
-      <c r="B404" s="6" t="s">
+      <c r="C404" s="6" t="s">
         <v>1461</v>
-      </c>
-      <c r="C404" s="6" t="s">
-        <v>1462</v>
       </c>
       <c r="D404" s="6"/>
       <c r="E404" s="6"/>
@@ -19824,13 +19826,13 @@
     </row>
     <row r="405" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A405" s="12" t="s">
+        <v>1462</v>
+      </c>
+      <c r="B405" s="6" t="s">
         <v>1463</v>
       </c>
-      <c r="B405" s="6" t="s">
+      <c r="C405" s="6" t="s">
         <v>1464</v>
-      </c>
-      <c r="C405" s="6" t="s">
-        <v>1465</v>
       </c>
       <c r="D405" s="6"/>
       <c r="E405" s="6"/>
@@ -19858,13 +19860,13 @@
     </row>
     <row r="406" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A406" s="12" t="s">
+        <v>1465</v>
+      </c>
+      <c r="B406" s="6" t="s">
         <v>1466</v>
       </c>
-      <c r="B406" s="6" t="s">
+      <c r="C406" s="6" t="s">
         <v>1467</v>
-      </c>
-      <c r="C406" s="6" t="s">
-        <v>1468</v>
       </c>
       <c r="D406" s="6"/>
       <c r="E406" s="6"/>
@@ -19892,13 +19894,13 @@
     </row>
     <row r="407" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A407" s="12" t="s">
+        <v>1468</v>
+      </c>
+      <c r="B407" s="6" t="s">
         <v>1469</v>
       </c>
-      <c r="B407" s="6" t="s">
+      <c r="C407" s="6" t="s">
         <v>1470</v>
-      </c>
-      <c r="C407" s="6" t="s">
-        <v>1471</v>
       </c>
       <c r="D407" s="6"/>
       <c r="E407" s="6"/>
@@ -19926,13 +19928,13 @@
     </row>
     <row r="408" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A408" s="12" t="s">
+        <v>1471</v>
+      </c>
+      <c r="B408" s="6" t="s">
         <v>1472</v>
       </c>
-      <c r="B408" s="6" t="s">
+      <c r="C408" s="6" t="s">
         <v>1473</v>
-      </c>
-      <c r="C408" s="6" t="s">
-        <v>1474</v>
       </c>
       <c r="D408" s="6"/>
       <c r="E408" s="6"/>
@@ -19960,13 +19962,13 @@
     </row>
     <row r="409" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A409" s="12" t="s">
+        <v>1474</v>
+      </c>
+      <c r="B409" s="6" t="s">
         <v>1475</v>
       </c>
-      <c r="B409" s="6" t="s">
+      <c r="C409" s="6" t="s">
         <v>1476</v>
-      </c>
-      <c r="C409" s="6" t="s">
-        <v>1477</v>
       </c>
       <c r="D409" s="6"/>
       <c r="E409" s="6"/>
@@ -19994,13 +19996,13 @@
     </row>
     <row r="410" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A410" s="12" t="s">
+        <v>1477</v>
+      </c>
+      <c r="B410" s="6" t="s">
         <v>1478</v>
       </c>
-      <c r="B410" s="6" t="s">
+      <c r="C410" s="6" t="s">
         <v>1479</v>
-      </c>
-      <c r="C410" s="6" t="s">
-        <v>1480</v>
       </c>
       <c r="D410" s="6"/>
       <c r="E410" s="6"/>
@@ -20028,13 +20030,13 @@
     </row>
     <row r="411" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A411" s="12" t="s">
+        <v>1480</v>
+      </c>
+      <c r="B411" s="6" t="s">
         <v>1481</v>
       </c>
-      <c r="B411" s="6" t="s">
+      <c r="C411" s="6" t="s">
         <v>1482</v>
-      </c>
-      <c r="C411" s="6" t="s">
-        <v>1483</v>
       </c>
       <c r="D411" s="6"/>
       <c r="E411" s="6"/>
@@ -20062,13 +20064,13 @@
     </row>
     <row r="412" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A412" s="12" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B412" s="6" t="s">
         <v>1484</v>
       </c>
-      <c r="B412" s="6" t="s">
+      <c r="C412" s="6" t="s">
         <v>1485</v>
-      </c>
-      <c r="C412" s="6" t="s">
-        <v>1486</v>
       </c>
       <c r="D412" s="6"/>
       <c r="E412" s="6"/>
@@ -20096,13 +20098,13 @@
     </row>
     <row r="413" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A413" s="12" t="s">
+        <v>1486</v>
+      </c>
+      <c r="B413" s="6" t="s">
         <v>1487</v>
       </c>
-      <c r="B413" s="6" t="s">
+      <c r="C413" s="6" t="s">
         <v>1488</v>
-      </c>
-      <c r="C413" s="6" t="s">
-        <v>1489</v>
       </c>
       <c r="D413" s="6"/>
       <c r="E413" s="6"/>
@@ -20130,13 +20132,13 @@
     </row>
     <row r="414" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A414" s="12" t="s">
+        <v>1489</v>
+      </c>
+      <c r="B414" s="6" t="s">
         <v>1490</v>
       </c>
-      <c r="B414" s="6" t="s">
+      <c r="C414" s="6" t="s">
         <v>1491</v>
-      </c>
-      <c r="C414" s="6" t="s">
-        <v>1492</v>
       </c>
       <c r="D414" s="6"/>
       <c r="E414" s="6"/>
@@ -20198,13 +20200,13 @@
     </row>
     <row r="416" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A416" s="12" t="s">
+        <v>1492</v>
+      </c>
+      <c r="B416" s="6" t="s">
         <v>1493</v>
       </c>
-      <c r="B416" s="6" t="s">
+      <c r="C416" s="6" t="s">
         <v>1494</v>
-      </c>
-      <c r="C416" s="6" t="s">
-        <v>1495</v>
       </c>
       <c r="D416" s="6"/>
       <c r="E416" s="6"/>
@@ -20232,13 +20234,13 @@
     </row>
     <row r="417" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A417" s="12" t="s">
+        <v>1495</v>
+      </c>
+      <c r="B417" s="6" t="s">
         <v>1496</v>
       </c>
-      <c r="B417" s="6" t="s">
+      <c r="C417" s="6" t="s">
         <v>1497</v>
-      </c>
-      <c r="C417" s="6" t="s">
-        <v>1498</v>
       </c>
       <c r="D417" s="6"/>
       <c r="E417" s="6"/>
@@ -20266,13 +20268,13 @@
     </row>
     <row r="418" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A418" s="12" t="s">
+        <v>1498</v>
+      </c>
+      <c r="B418" s="6" t="s">
         <v>1499</v>
       </c>
-      <c r="B418" s="6" t="s">
+      <c r="C418" s="6" t="s">
         <v>1500</v>
-      </c>
-      <c r="C418" s="6" t="s">
-        <v>1501</v>
       </c>
       <c r="D418" s="6"/>
       <c r="E418" s="6"/>
@@ -20334,13 +20336,13 @@
     </row>
     <row r="420" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A420" s="12" t="s">
+        <v>1501</v>
+      </c>
+      <c r="B420" s="6" t="s">
         <v>1502</v>
       </c>
-      <c r="B420" s="6" t="s">
+      <c r="C420" s="6" t="s">
         <v>1503</v>
-      </c>
-      <c r="C420" s="6" t="s">
-        <v>1504</v>
       </c>
       <c r="D420" s="6"/>
       <c r="E420" s="6"/>
@@ -20368,13 +20370,13 @@
     </row>
     <row r="421" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A421" s="12" t="s">
+        <v>1504</v>
+      </c>
+      <c r="B421" s="6" t="s">
         <v>1505</v>
       </c>
-      <c r="B421" s="6" t="s">
+      <c r="C421" s="6" t="s">
         <v>1506</v>
-      </c>
-      <c r="C421" s="6" t="s">
-        <v>1507</v>
       </c>
       <c r="D421" s="6"/>
       <c r="E421" s="6"/>
@@ -21388,13 +21390,13 @@
     </row>
     <row r="451" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A451" s="12" t="s">
+        <v>1507</v>
+      </c>
+      <c r="B451" s="6" t="s">
         <v>1508</v>
       </c>
-      <c r="B451" s="6" t="s">
+      <c r="C451" s="6" t="s">
         <v>1509</v>
-      </c>
-      <c r="C451" s="6" t="s">
-        <v>1510</v>
       </c>
       <c r="D451" s="6"/>
       <c r="E451" s="6"/>
@@ -21456,13 +21458,13 @@
     </row>
     <row r="453" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A453" s="12" t="s">
+        <v>1510</v>
+      </c>
+      <c r="B453" s="6" t="s">
         <v>1511</v>
       </c>
-      <c r="B453" s="6" t="s">
+      <c r="C453" s="6" t="s">
         <v>1512</v>
-      </c>
-      <c r="C453" s="6" t="s">
-        <v>1513</v>
       </c>
       <c r="D453" s="6"/>
       <c r="E453" s="6"/>
@@ -21490,13 +21492,13 @@
     </row>
     <row r="454" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A454" s="12" t="s">
+        <v>1513</v>
+      </c>
+      <c r="B454" s="6" t="s">
         <v>1514</v>
       </c>
-      <c r="B454" s="6" t="s">
+      <c r="C454" s="6" t="s">
         <v>1515</v>
-      </c>
-      <c r="C454" s="6" t="s">
-        <v>1516</v>
       </c>
       <c r="D454" s="6"/>
       <c r="E454" s="6"/>
@@ -21524,13 +21526,13 @@
     </row>
     <row r="455" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A455" s="12" t="s">
+        <v>1516</v>
+      </c>
+      <c r="B455" s="6" t="s">
         <v>1517</v>
       </c>
-      <c r="B455" s="6" t="s">
+      <c r="C455" s="6" t="s">
         <v>1518</v>
-      </c>
-      <c r="C455" s="6" t="s">
-        <v>1519</v>
       </c>
       <c r="D455" s="6"/>
       <c r="E455" s="6"/>
@@ -21558,13 +21560,13 @@
     </row>
     <row r="456" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A456" s="12" t="s">
+        <v>1519</v>
+      </c>
+      <c r="B456" s="6" t="s">
         <v>1520</v>
       </c>
-      <c r="B456" s="6" t="s">
+      <c r="C456" s="6" t="s">
         <v>1521</v>
-      </c>
-      <c r="C456" s="6" t="s">
-        <v>1522</v>
       </c>
       <c r="D456" s="6"/>
       <c r="E456" s="6"/>
@@ -21592,13 +21594,13 @@
     </row>
     <row r="457" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A457" s="12" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B457" s="6" t="s">
         <v>1523</v>
       </c>
-      <c r="B457" s="6" t="s">
+      <c r="C457" s="6" t="s">
         <v>1524</v>
-      </c>
-      <c r="C457" s="6" t="s">
-        <v>1525</v>
       </c>
       <c r="D457" s="6"/>
       <c r="E457" s="6"/>
@@ -21626,13 +21628,13 @@
     </row>
     <row r="458" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A458" s="12" t="s">
+        <v>1525</v>
+      </c>
+      <c r="B458" s="6" t="s">
         <v>1526</v>
       </c>
-      <c r="B458" s="6" t="s">
-        <v>1527</v>
-      </c>
       <c r="C458" s="6" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="D458" s="6"/>
       <c r="E458" s="6"/>
@@ -21660,13 +21662,13 @@
     </row>
     <row r="459" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A459" s="12" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B459" s="6" t="s">
         <v>1528</v>
       </c>
-      <c r="B459" s="6" t="s">
+      <c r="C459" s="6" t="s">
         <v>1529</v>
-      </c>
-      <c r="C459" s="6" t="s">
-        <v>1530</v>
       </c>
       <c r="D459" s="6"/>
       <c r="E459" s="6"/>
@@ -21728,13 +21730,13 @@
     </row>
     <row r="461" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A461" s="12" t="s">
+        <v>1530</v>
+      </c>
+      <c r="B461" s="6" t="s">
         <v>1531</v>
       </c>
-      <c r="B461" s="6" t="s">
+      <c r="C461" s="6" t="s">
         <v>1532</v>
-      </c>
-      <c r="C461" s="6" t="s">
-        <v>1533</v>
       </c>
       <c r="D461" s="6"/>
       <c r="E461" s="6"/>
@@ -21796,13 +21798,13 @@
     </row>
     <row r="463" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A463" s="12" t="s">
+        <v>1533</v>
+      </c>
+      <c r="B463" s="6" t="s">
         <v>1534</v>
       </c>
-      <c r="B463" s="6" t="s">
+      <c r="C463" s="6" t="s">
         <v>1535</v>
-      </c>
-      <c r="C463" s="6" t="s">
-        <v>1536</v>
       </c>
       <c r="D463" s="6"/>
       <c r="E463" s="6"/>
@@ -21830,13 +21832,13 @@
     </row>
     <row r="464" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A464" s="12" t="s">
+        <v>1536</v>
+      </c>
+      <c r="B464" s="6" t="s">
         <v>1537</v>
       </c>
-      <c r="B464" s="6" t="s">
+      <c r="C464" s="6" t="s">
         <v>1538</v>
-      </c>
-      <c r="C464" s="6" t="s">
-        <v>1539</v>
       </c>
       <c r="D464" s="6"/>
       <c r="E464" s="6"/>
@@ -21864,13 +21866,13 @@
     </row>
     <row r="465" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A465" s="12" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B465" s="6" t="s">
         <v>1540</v>
       </c>
-      <c r="B465" s="6" t="s">
+      <c r="C465" s="6" t="s">
         <v>1541</v>
-      </c>
-      <c r="C465" s="6" t="s">
-        <v>1542</v>
       </c>
       <c r="D465" s="6"/>
       <c r="E465" s="6"/>
@@ -21898,13 +21900,13 @@
     </row>
     <row r="466" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A466" s="12" t="s">
+        <v>1542</v>
+      </c>
+      <c r="B466" s="6" t="s">
         <v>1543</v>
       </c>
-      <c r="B466" s="6" t="s">
+      <c r="C466" s="6" t="s">
         <v>1544</v>
-      </c>
-      <c r="C466" s="6" t="s">
-        <v>1545</v>
       </c>
       <c r="D466" s="6"/>
       <c r="E466" s="6"/>
@@ -21932,13 +21934,13 @@
     </row>
     <row r="467" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A467" s="12" t="s">
+        <v>1545</v>
+      </c>
+      <c r="B467" s="6" t="s">
         <v>1546</v>
       </c>
-      <c r="B467" s="6" t="s">
+      <c r="C467" s="6" t="s">
         <v>1547</v>
-      </c>
-      <c r="C467" s="6" t="s">
-        <v>1548</v>
       </c>
       <c r="D467" s="6"/>
       <c r="E467" s="6"/>
@@ -21966,13 +21968,13 @@
     </row>
     <row r="468" spans="1:26" ht="16" x14ac:dyDescent="0.25">
       <c r="A468" s="12" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B468" s="6" t="s">
+        <v>1548</v>
+      </c>
+      <c r="C468" s="6" t="s">
         <v>1549</v>
-      </c>
-      <c r="C468" s="6" t="s">
-        <v>1550</v>
       </c>
       <c r="D468" s="6"/>
       <c r="E468" s="6"/>

</xml_diff>